<commit_message>
Add Semua tentang password.txt - 08.59
</commit_message>
<xml_diff>
--- a/2018-September/From Email & WhatsApp - Project Mandiri/DCTM Doc Type and Metadata-V.04.xlsx
+++ b/2018-September/From Email & WhatsApp - Project Mandiri/DCTM Doc Type and Metadata-V.04.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DailyMonthlyLog\2018-September\From Email &amp; WhatsApp - Project Mandiri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93A7EF6-1705-4EB8-ACDF-CA585A9A1B0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6C7961-0435-402D-93EC-EBB3C1B6E685}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="6165" tabRatio="725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="153">
   <si>
     <t>No.</t>
   </si>
@@ -426,6 +426,66 @@
   </si>
   <si>
     <t>List Attachment Dokumen</t>
+  </si>
+  <si>
+    <t>LENGTH</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>DATE/TIME</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ATTRIBUTE/METADATA IN REPO</t>
+  </si>
+  <si>
+    <t>attr_sme_main_name</t>
+  </si>
+  <si>
+    <t>attr_sme_main_app</t>
+  </si>
+  <si>
+    <t>attr_surround_app_1</t>
+  </si>
+  <si>
+    <t>attr_surround_app_2</t>
+  </si>
+  <si>
+    <t>attr_surround_app_3</t>
+  </si>
+  <si>
+    <t>attr_surround_app_4</t>
+  </si>
+  <si>
+    <t>attr_surround_app_5</t>
+  </si>
+  <si>
+    <t>attr_sme_name_1</t>
+  </si>
+  <si>
+    <t>attr_sme_name_2</t>
+  </si>
+  <si>
+    <t>attr_sme_name_3</t>
+  </si>
+  <si>
+    <t>attr_sme_name_4</t>
+  </si>
+  <si>
+    <t>attr_sme_name_5</t>
+  </si>
+  <si>
+    <t>attr_review_d_from</t>
+  </si>
+  <si>
+    <t>attr_review_d_to</t>
+  </si>
+  <si>
+    <t>attr_revisi_need</t>
+  </si>
+  <si>
+    <t>attr_reviewer_name</t>
   </si>
 </sst>
 </file>
@@ -546,7 +606,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -1097,6 +1157,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="8"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1105,7 +1178,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1310,15 +1383,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1329,6 +1393,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6528,25 +6631,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:G73"/>
+  <dimension ref="A3:I73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" style="25" customWidth="1"/>
     <col min="3" max="3" width="38" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32" style="25" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="71.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="25"/>
+    <col min="4" max="4" width="38" style="25" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" style="25" customWidth="1"/>
+    <col min="6" max="6" width="32" style="25" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="71.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>7</v>
       </c>
@@ -6557,30 +6662,38 @@
         <v>22</v>
       </c>
       <c r="D3" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="H3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="I3" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="59"/>
       <c r="C4" s="61"/>
       <c r="D4" s="76"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="72" t="s">
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="72" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>1</v>
       </c>
@@ -6590,101 +6703,125 @@
       <c r="C5" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="58" t="s">
+      <c r="D5" s="30"/>
+      <c r="E5" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="83">
+        <v>50</v>
+      </c>
+      <c r="G5" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="H5" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="73"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5" s="73"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
       <c r="B6" s="36"/>
       <c r="C6" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="58"/>
-      <c r="F6" s="29" t="s">
+      <c r="D6" s="30"/>
+      <c r="E6" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" s="83" t="s">
+        <v>134</v>
+      </c>
+      <c r="G6" s="58"/>
+      <c r="H6" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="73"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" s="73"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
       <c r="B7" s="36"/>
       <c r="C7" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="30"/>
+      <c r="E7" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="83">
+        <v>225</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="73"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" s="73"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
       <c r="B8" s="36"/>
       <c r="C8" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="30"/>
+      <c r="E8" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="83">
+        <v>20</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="73"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8" s="73"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
       <c r="B9" s="36"/>
       <c r="C9" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="30"/>
+      <c r="E9" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="83">
+        <v>20</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="73"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I9" s="73"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="53"/>
       <c r="B10" s="60"/>
       <c r="C10" s="54"/>
       <c r="D10" s="54"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="74"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="54"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="74"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="69"/>
       <c r="C11" s="65" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="77"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="66" t="s">
+      <c r="E11" s="77"/>
+      <c r="F11" s="85"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="75" t="s">
+      <c r="I11" s="75" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>2</v>
       </c>
@@ -6694,89 +6831,111 @@
       <c r="C12" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="58" t="s">
+      <c r="D12" s="77"/>
+      <c r="E12" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="83">
+        <v>50</v>
+      </c>
+      <c r="G12" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="29" t="s">
+      <c r="H12" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="G12" s="73"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I12" s="73"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="36"/>
       <c r="C13" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="82"/>
+      <c r="E13" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="29" t="s">
+      <c r="F13" s="83" t="s">
+        <v>134</v>
+      </c>
+      <c r="G13" s="16"/>
+      <c r="H13" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="G13" s="73"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I13" s="73"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="36"/>
       <c r="C14" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="30"/>
+      <c r="E14" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="83">
+        <v>225</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="G14" s="73"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I14" s="73"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="36"/>
       <c r="C15" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="30"/>
+      <c r="E15" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="67"/>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="83">
+        <v>20</v>
+      </c>
+      <c r="G15" s="67"/>
+      <c r="H15" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="G15" s="73"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I15" s="73"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" s="62"/>
       <c r="C16" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="30"/>
+      <c r="E16" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="83">
+        <v>20</v>
+      </c>
+      <c r="G16" s="19"/>
+      <c r="H16" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="G16" s="74"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16" s="74"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
       <c r="B17" s="68"/>
       <c r="C17" s="21"/>
       <c r="D17" s="21"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="75" t="s">
+      <c r="E17" s="21"/>
+      <c r="F17" s="88"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="75" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>3</v>
       </c>
@@ -6786,77 +6945,95 @@
       <c r="C18" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="E18" s="58" t="s">
+      <c r="D18" s="30"/>
+      <c r="E18" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="83">
+        <v>50</v>
+      </c>
+      <c r="G18" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="34" t="s">
+      <c r="H18" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="73"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18" s="73"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" s="36"/>
       <c r="C19" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="30"/>
+      <c r="E19" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="E19" s="16"/>
-      <c r="F19" s="29" t="s">
+      <c r="F19" s="83" t="s">
+        <v>134</v>
+      </c>
+      <c r="G19" s="16"/>
+      <c r="H19" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="73"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19" s="73"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
       <c r="B20" s="36"/>
       <c r="C20" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="30"/>
+      <c r="E20" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="16"/>
-      <c r="F20" s="29" t="s">
+      <c r="F20" s="83">
+        <v>20</v>
+      </c>
+      <c r="G20" s="16"/>
+      <c r="H20" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="G20" s="73"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20" s="73"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
       <c r="B21" s="36"/>
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="73"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="30"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="73"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="53"/>
       <c r="B22" s="60"/>
       <c r="C22" s="57"/>
       <c r="D22" s="57"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="74"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="57"/>
+      <c r="F22" s="84"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="74"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="20"/>
       <c r="B23" s="68"/>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="75" t="s">
+      <c r="E23" s="21"/>
+      <c r="F23" s="88"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="75" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>4</v>
       </c>
@@ -6866,295 +7043,451 @@
       <c r="C24" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="D24" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="E24" s="58" t="s">
+      <c r="D24" s="30"/>
+      <c r="E24" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="83">
+        <v>50</v>
+      </c>
+      <c r="G24" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="34" t="s">
+      <c r="H24" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="G24" s="73"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I24" s="73"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="36"/>
       <c r="C25" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="D25" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="58" t="s">
+      <c r="D25" s="30"/>
+      <c r="E25" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" s="83">
+        <v>20</v>
+      </c>
+      <c r="G25" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="29" t="s">
+      <c r="H25" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="G25" s="73"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I25" s="73"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="36"/>
       <c r="C26" s="30" t="s">
         <v>89</v>
       </c>
       <c r="D26" s="30"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="29" t="s">
+      <c r="E26" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="83">
+        <v>50</v>
+      </c>
+      <c r="G26" s="16"/>
+      <c r="H26" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="G26" s="73"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I26" s="73"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="36"/>
       <c r="C27" s="30" t="s">
         <v>90</v>
       </c>
       <c r="D27" s="30"/>
-      <c r="E27" s="58" t="s">
+      <c r="E27" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" s="83">
+        <v>50</v>
+      </c>
+      <c r="G27" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="29" t="s">
+      <c r="H27" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="G27" s="73"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I27" s="73"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
       <c r="B28" s="36"/>
       <c r="C28" s="30" t="s">
         <v>91</v>
       </c>
       <c r="D28" s="30"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="29" t="s">
+      <c r="E28" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" s="83">
+        <v>225</v>
+      </c>
+      <c r="G28" s="16"/>
+      <c r="H28" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="G28" s="73"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I28" s="73"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" s="36"/>
       <c r="C29" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="D29" s="30"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="29" t="s">
+      <c r="D29" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F29" s="83">
+        <v>50</v>
+      </c>
+      <c r="G29" s="16"/>
+      <c r="H29" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="G29" s="73"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I29" s="73"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
       <c r="B30" s="36"/>
       <c r="C30" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="D30" s="30"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="29" t="s">
+      <c r="D30" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" s="83">
+        <v>100</v>
+      </c>
+      <c r="G30" s="16"/>
+      <c r="H30" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="G30" s="73"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I30" s="73"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
       <c r="B31" s="36"/>
       <c r="C31" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="D31" s="30"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="29" t="s">
+      <c r="D31" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="E31" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F31" s="83">
+        <v>50</v>
+      </c>
+      <c r="G31" s="16"/>
+      <c r="H31" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="G31" s="73"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I31" s="73"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
       <c r="B32" s="36"/>
       <c r="C32" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="D32" s="30"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="29" t="s">
+      <c r="D32" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="E32" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F32" s="83">
+        <v>100</v>
+      </c>
+      <c r="G32" s="16"/>
+      <c r="H32" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="G32" s="73"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I32" s="73"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
       <c r="B33" s="36"/>
       <c r="C33" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="D33" s="30"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="29" t="s">
+      <c r="D33" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="E33" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F33" s="83">
+        <v>50</v>
+      </c>
+      <c r="G33" s="16"/>
+      <c r="H33" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="G33" s="73"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I33" s="73"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="15"/>
       <c r="B34" s="36"/>
       <c r="C34" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="D34" s="30"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="29" t="s">
+      <c r="D34" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F34" s="83">
+        <v>100</v>
+      </c>
+      <c r="G34" s="16"/>
+      <c r="H34" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="G34" s="73"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I34" s="73"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
       <c r="B35" s="36"/>
       <c r="C35" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="D35" s="30"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="29" t="s">
+      <c r="D35" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="E35" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F35" s="83">
+        <v>50</v>
+      </c>
+      <c r="G35" s="16"/>
+      <c r="H35" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G35" s="73"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I35" s="73"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="15"/>
       <c r="B36" s="36"/>
       <c r="C36" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="D36" s="30"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="29" t="s">
+      <c r="D36" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F36" s="83">
+        <v>100</v>
+      </c>
+      <c r="G36" s="16"/>
+      <c r="H36" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G36" s="73"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I36" s="73"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="15"/>
       <c r="B37" s="36"/>
       <c r="C37" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="D37" s="30"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="29" t="s">
+      <c r="D37" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" s="83">
+        <v>50</v>
+      </c>
+      <c r="G37" s="16"/>
+      <c r="H37" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="G37" s="73"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I37" s="73"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
       <c r="B38" s="36"/>
       <c r="C38" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="D38" s="30"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="29" t="s">
+      <c r="D38" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F38" s="83">
+        <v>100</v>
+      </c>
+      <c r="G38" s="16"/>
+      <c r="H38" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="G38" s="73"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I38" s="73"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
       <c r="B39" s="36"/>
       <c r="C39" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="D39" s="30"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="29" t="s">
+      <c r="D39" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="E39" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F39" s="83">
+        <v>50</v>
+      </c>
+      <c r="G39" s="16"/>
+      <c r="H39" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G39" s="73"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I39" s="73"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
       <c r="B40" s="36"/>
       <c r="C40" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="D40" s="30"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="29" t="s">
+      <c r="D40" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E40" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F40" s="83">
+        <v>100</v>
+      </c>
+      <c r="G40" s="16"/>
+      <c r="H40" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="G40" s="73"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I40" s="73"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="15"/>
       <c r="B41" s="36"/>
       <c r="C41" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="D41" s="30"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="29" t="s">
+      <c r="D41" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="E41" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F41" s="83">
+        <v>50</v>
+      </c>
+      <c r="G41" s="16"/>
+      <c r="H41" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="G41" s="73"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I41" s="73"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="15"/>
       <c r="B42" s="36"/>
       <c r="C42" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="D42" s="30"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="29" t="s">
+      <c r="D42" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="E42" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F42" s="83">
+        <v>50</v>
+      </c>
+      <c r="G42" s="16"/>
+      <c r="H42" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="G42" s="73"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I42" s="73"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="15"/>
       <c r="B43" s="36"/>
       <c r="C43" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="D43" s="30"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="29" t="s">
+      <c r="D43" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="E43" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F43" s="83">
+        <v>50</v>
+      </c>
+      <c r="G43" s="16"/>
+      <c r="H43" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="G43" s="73"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I43" s="73"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="53"/>
       <c r="B44" s="60"/>
-      <c r="C44" s="81" t="s">
+      <c r="C44" s="78" t="s">
         <v>102</v>
       </c>
-      <c r="D44" s="57"/>
-      <c r="E44" s="55"/>
-      <c r="F44" s="82" t="s">
+      <c r="D44" s="78" t="s">
+        <v>152</v>
+      </c>
+      <c r="E44" s="78" t="s">
+        <v>64</v>
+      </c>
+      <c r="F44" s="91">
+        <v>50</v>
+      </c>
+      <c r="G44" s="55"/>
+      <c r="H44" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="G44" s="74"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I44" s="74"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="15"/>
       <c r="B45" s="28"/>
       <c r="C45" s="24"/>
       <c r="D45" s="24"/>
-      <c r="E45" s="23"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="75" t="s">
+      <c r="E45" s="24"/>
+      <c r="F45" s="87"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="75" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <v>5</v>
       </c>
@@ -7164,74 +7497,88 @@
       <c r="C46" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D46" s="30" t="s">
+      <c r="D46" s="30"/>
+      <c r="E46" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="E46" s="16"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="73"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F46" s="83"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="73"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="15"/>
       <c r="B47" s="28"/>
       <c r="C47" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D47" s="30" t="s">
+      <c r="D47" s="30"/>
+      <c r="E47" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="E47" s="16"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="73"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F47" s="83"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="73"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="15"/>
       <c r="B48" s="28"/>
       <c r="C48" s="30"/>
       <c r="D48" s="30"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="73"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E48" s="30"/>
+      <c r="F48" s="83"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="29"/>
+      <c r="I48" s="73"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="15"/>
       <c r="B49" s="28"/>
       <c r="C49" s="30"/>
       <c r="D49" s="30"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="29"/>
-      <c r="G49" s="73"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E49" s="30"/>
+      <c r="F49" s="83"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="73"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="15"/>
       <c r="B50" s="28"/>
       <c r="C50" s="26"/>
       <c r="D50" s="26"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="73"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E50" s="26"/>
+      <c r="F50" s="86"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="27"/>
+      <c r="I50" s="73"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="17"/>
       <c r="B51" s="31"/>
       <c r="C51" s="18"/>
       <c r="D51" s="18"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="74"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E51" s="18"/>
+      <c r="F51" s="89"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="32"/>
+      <c r="I51" s="74"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="20"/>
       <c r="B52" s="68"/>
       <c r="C52" s="21"/>
       <c r="D52" s="21"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="33"/>
-      <c r="G52" s="75" t="s">
+      <c r="E52" s="21"/>
+      <c r="F52" s="88"/>
+      <c r="G52" s="22"/>
+      <c r="H52" s="33"/>
+      <c r="I52" s="75" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <v>6</v>
       </c>
@@ -7241,67 +7588,79 @@
       <c r="C53" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D53" s="30" t="s">
+      <c r="D53" s="30"/>
+      <c r="E53" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="E53" s="58" t="s">
+      <c r="F53" s="83"/>
+      <c r="G53" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="F53" s="34"/>
-      <c r="G53" s="73"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53" s="34"/>
+      <c r="I53" s="73"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="15"/>
       <c r="B54" s="36"/>
       <c r="C54" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D54" s="30" t="s">
+      <c r="D54" s="30"/>
+      <c r="E54" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="E54" s="16"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="73"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F54" s="83"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="29"/>
+      <c r="I54" s="73"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="15"/>
       <c r="B55" s="36"/>
       <c r="C55" s="30"/>
       <c r="D55" s="30"/>
-      <c r="E55" s="16"/>
-      <c r="F55" s="29"/>
-      <c r="G55" s="73"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E55" s="30"/>
+      <c r="F55" s="83"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="29"/>
+      <c r="I55" s="73"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="15"/>
       <c r="B56" s="36"/>
       <c r="C56" s="30"/>
       <c r="D56" s="30"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="29"/>
-      <c r="G56" s="73"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E56" s="30"/>
+      <c r="F56" s="83"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="29"/>
+      <c r="I56" s="73"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="53"/>
       <c r="B57" s="60"/>
       <c r="C57" s="57"/>
       <c r="D57" s="57"/>
-      <c r="E57" s="55"/>
-      <c r="F57" s="82"/>
-      <c r="G57" s="74"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E57" s="57"/>
+      <c r="F57" s="84"/>
+      <c r="G57" s="55"/>
+      <c r="H57" s="79"/>
+      <c r="I57" s="74"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="20"/>
       <c r="B58" s="68"/>
       <c r="C58" s="21"/>
       <c r="D58" s="21"/>
-      <c r="E58" s="83"/>
-      <c r="F58" s="30"/>
-      <c r="G58" s="84" t="s">
+      <c r="E58" s="21"/>
+      <c r="F58" s="90"/>
+      <c r="G58" s="80"/>
+      <c r="H58" s="30"/>
+      <c r="I58" s="81" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <v>7</v>
       </c>
@@ -7311,206 +7670,236 @@
       <c r="C59" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="D59" s="30" t="s">
+      <c r="D59" s="24"/>
+      <c r="E59" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="E59" s="58" t="s">
+      <c r="F59" s="83"/>
+      <c r="G59" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="F59" s="35" t="s">
+      <c r="H59" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="G59" s="73"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I59" s="73"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="15"/>
       <c r="B60" s="36"/>
       <c r="C60" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="D60" s="30" t="s">
+      <c r="D60" s="30"/>
+      <c r="E60" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="E60" s="58" t="s">
+      <c r="F60" s="83"/>
+      <c r="G60" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="F60" s="34" t="s">
+      <c r="H60" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="G60" s="73"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I60" s="73"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="15"/>
       <c r="B61" s="36"/>
       <c r="C61" s="30" t="s">
         <v>106</v>
       </c>
       <c r="D61" s="30"/>
-      <c r="E61" s="58" t="s">
+      <c r="E61" s="30"/>
+      <c r="F61" s="83"/>
+      <c r="G61" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="F61" s="29" t="s">
+      <c r="H61" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="G61" s="73"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I61" s="73"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="15"/>
       <c r="B62" s="36"/>
       <c r="C62" s="30" t="s">
         <v>107</v>
       </c>
       <c r="D62" s="30"/>
-      <c r="E62" s="58" t="s">
+      <c r="E62" s="30"/>
+      <c r="F62" s="83"/>
+      <c r="G62" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="F62" s="29" t="s">
+      <c r="H62" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="G62" s="73"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I62" s="73"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="15"/>
       <c r="B63" s="36"/>
       <c r="C63" s="30" t="s">
         <v>108</v>
       </c>
       <c r="D63" s="30"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="29" t="s">
+      <c r="E63" s="30"/>
+      <c r="F63" s="83"/>
+      <c r="G63" s="16"/>
+      <c r="H63" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="G63" s="73"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I63" s="73"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="15"/>
       <c r="B64" s="36"/>
       <c r="C64" s="30" t="s">
         <v>109</v>
       </c>
       <c r="D64" s="30"/>
-      <c r="E64" s="16"/>
-      <c r="F64" s="29" t="s">
+      <c r="E64" s="30"/>
+      <c r="F64" s="83"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="G64" s="73"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I64" s="73"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="15"/>
       <c r="B65" s="36"/>
       <c r="C65" s="30" t="s">
         <v>110</v>
       </c>
       <c r="D65" s="30"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="29" t="s">
+      <c r="E65" s="30"/>
+      <c r="F65" s="83"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="G65" s="73"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I65" s="73"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="15"/>
       <c r="B66" s="36"/>
       <c r="C66" s="30" t="s">
         <v>44</v>
       </c>
       <c r="D66" s="30"/>
-      <c r="E66" s="16"/>
-      <c r="F66" s="29" t="s">
+      <c r="E66" s="30"/>
+      <c r="F66" s="83"/>
+      <c r="G66" s="16"/>
+      <c r="H66" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="G66" s="73"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I66" s="73"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="15"/>
       <c r="B67" s="36"/>
       <c r="C67" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="D67" s="30"/>
-      <c r="E67" s="16"/>
-      <c r="F67" s="29" t="s">
+      <c r="D67" s="24"/>
+      <c r="E67" s="30"/>
+      <c r="F67" s="83"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="G67" s="73"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I67" s="73"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="15"/>
       <c r="B68" s="36"/>
       <c r="C68" s="30" t="s">
         <v>112</v>
       </c>
       <c r="D68" s="30"/>
-      <c r="E68" s="16"/>
-      <c r="F68" s="29" t="s">
+      <c r="E68" s="30"/>
+      <c r="F68" s="83"/>
+      <c r="G68" s="16"/>
+      <c r="H68" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="G68" s="73"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I68" s="73"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="15"/>
       <c r="B69" s="36"/>
       <c r="C69" s="30" t="s">
         <v>113</v>
       </c>
       <c r="D69" s="30"/>
-      <c r="E69" s="16"/>
-      <c r="F69" s="29" t="s">
+      <c r="E69" s="30"/>
+      <c r="F69" s="83"/>
+      <c r="G69" s="16"/>
+      <c r="H69" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="G69" s="73"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I69" s="73"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="15"/>
       <c r="B70" s="36"/>
       <c r="C70" s="30" t="s">
         <v>114</v>
       </c>
       <c r="D70" s="30"/>
-      <c r="E70" s="16"/>
-      <c r="F70" s="29" t="s">
+      <c r="E70" s="30"/>
+      <c r="F70" s="83"/>
+      <c r="G70" s="16"/>
+      <c r="H70" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="G70" s="73"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I70" s="73"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="15"/>
       <c r="B71" s="36"/>
       <c r="C71" s="30" t="s">
         <v>115</v>
       </c>
       <c r="D71" s="30"/>
-      <c r="E71" s="16"/>
-      <c r="F71" s="29" t="s">
+      <c r="E71" s="30"/>
+      <c r="F71" s="83"/>
+      <c r="G71" s="16"/>
+      <c r="H71" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="G71" s="73"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I71" s="73"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="15"/>
       <c r="B72" s="36"/>
       <c r="C72" s="30" t="s">
         <v>116</v>
       </c>
       <c r="D72" s="30"/>
-      <c r="E72" s="16"/>
-      <c r="F72" s="29" t="s">
+      <c r="E72" s="30"/>
+      <c r="F72" s="83"/>
+      <c r="G72" s="16"/>
+      <c r="H72" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="G72" s="73"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I72" s="73"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="53"/>
       <c r="B73" s="60"/>
       <c r="C73" s="57" t="s">
         <v>117</v>
       </c>
       <c r="D73" s="57"/>
-      <c r="E73" s="55"/>
-      <c r="F73" s="56" t="s">
+      <c r="E73" s="57"/>
+      <c r="F73" s="84"/>
+      <c r="G73" s="55"/>
+      <c r="H73" s="56" t="s">
         <v>132</v>
       </c>
-      <c r="G73" s="74"/>
+      <c r="I73" s="74"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7652,13 +8041,13 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="F2" s="78" t="s">
+      <c r="F2" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="80"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="93"/>
+      <c r="J2" s="94"/>
     </row>
     <row r="3" spans="1:13" ht="86.25" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">

</xml_diff>